<commit_message>
work on SWL check
</commit_message>
<xml_diff>
--- a/python/node_types.xlsx
+++ b/python/node_types.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27715"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/ABOS/Prawler/cable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/GitHub/sots-cable-model/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D057A531-FE18-B94B-AAED-BA48B9DB1234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10840" yWindow="1800" windowWidth="25440" windowHeight="21320"/>
+    <workbookView xWindow="10840" yWindow="1800" windowWidth="25440" windowHeight="21320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="node_types_2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="90">
   <si>
     <t>Crosby 3/4</t>
   </si>
@@ -302,7 +314,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -782,7 +794,7 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1145,11 +1157,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1235,7 +1247,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="2">
-        <f t="shared" ref="H2:H39" si="0">D2*9.81*G2</f>
+        <f t="shared" ref="H2:H37" si="0">D2*9.81*G2</f>
         <v>0</v>
       </c>
       <c r="I2">
@@ -2199,7 +2211,7 @@
         <v>6890</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" ref="D20:D33" si="1">C20*E20</f>
+        <f t="shared" ref="D20:D31" si="1">C20*E20</f>
         <v>34450</v>
       </c>
       <c r="E20">
@@ -2446,7 +2458,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>2</v>
@@ -2484,10 +2496,10 @@
         <v>0</v>
       </c>
       <c r="M24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O24">
         <v>1</v>
@@ -2505,7 +2517,7 @@
         <v>0</v>
       </c>
       <c r="T24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
@@ -2513,27 +2525,27 @@
         <v>47</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C25" s="2">
-        <v>6500</v>
+        <v>5440</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="1"/>
-        <v>39000</v>
+        <v>27200</v>
       </c>
       <c r="E25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="G25">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="H25" s="2">
         <f t="shared" si="0"/>
-        <v>573885</v>
+        <v>453614.39999999997</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -2574,30 +2586,30 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C26" s="2">
-        <v>5440</v>
+        <v>4750</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="1"/>
-        <v>27200</v>
+        <v>28500</v>
       </c>
       <c r="E26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F26">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="G26">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" si="0"/>
-        <v>453614.39999999997</v>
+        <v>419377.5</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -2618,10 +2630,10 @@
         <v>0</v>
       </c>
       <c r="O26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q26">
         <v>0</v>
@@ -2633,7 +2645,7 @@
         <v>0</v>
       </c>
       <c r="T26" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
@@ -2641,27 +2653,27 @@
         <v>49</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C27" s="2">
-        <v>4750</v>
+        <v>5440</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="1"/>
-        <v>28500</v>
+        <v>27200</v>
       </c>
       <c r="E27">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="G27">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" si="0"/>
-        <v>419377.5</v>
+        <v>453614.39999999997</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -2702,45 +2714,36 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C28" s="2">
-        <v>5440</v>
+        <v>4750</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="1"/>
-        <v>27200</v>
+        <v>28500</v>
       </c>
       <c r="E28">
-        <v>5</v>
-      </c>
-      <c r="F28">
-        <v>3.8</v>
-      </c>
-      <c r="G28">
-        <v>1.7</v>
+        <v>6</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" si="0"/>
-        <v>453614.39999999997</v>
+        <v>0</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28">
         <v>0</v>
       </c>
       <c r="K28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28">
         <v>0</v>
       </c>
       <c r="M28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N28">
         <v>0</v>
@@ -2766,10 +2769,7 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C29" s="2">
         <v>5440</v>
@@ -2781,30 +2781,24 @@
       <c r="E29">
         <v>5</v>
       </c>
-      <c r="F29">
-        <v>3.7</v>
-      </c>
-      <c r="G29">
-        <v>2.25</v>
-      </c>
       <c r="H29" s="2">
         <f t="shared" si="0"/>
-        <v>600372</v>
+        <v>0</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29">
         <v>0</v>
       </c>
       <c r="K29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L29">
         <v>0</v>
       </c>
       <c r="M29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N29">
         <v>0</v>
@@ -2830,7 +2824,7 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C30" s="2">
         <v>4750</v>
@@ -2885,7 +2879,7 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C31" s="2">
         <v>5440</v>
@@ -2940,21 +2934,30 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>81</v>
+      </c>
+      <c r="B32" t="s">
+        <v>84</v>
       </c>
       <c r="C32" s="2">
-        <v>4750</v>
+        <v>3250</v>
       </c>
       <c r="D32" s="2">
-        <f t="shared" si="1"/>
-        <v>28500</v>
+        <f t="shared" ref="D32:D33" si="2">C32*E32</f>
+        <v>19500</v>
       </c>
       <c r="E32">
         <v>6</v>
       </c>
+      <c r="F32">
+        <v>3.7</v>
+      </c>
+      <c r="G32">
+        <v>1.5</v>
+      </c>
       <c r="H32" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="H32:H33" si="3">D32*9.81*G32</f>
+        <v>286942.5</v>
       </c>
       <c r="I32">
         <v>1</v>
@@ -2988,28 +2991,34 @@
       </c>
       <c r="S32">
         <v>0</v>
-      </c>
-      <c r="T32" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>81</v>
+      </c>
+      <c r="B33" t="s">
+        <v>85</v>
       </c>
       <c r="C33" s="2">
-        <v>5440</v>
+        <v>1910</v>
       </c>
       <c r="D33" s="2">
-        <f t="shared" si="1"/>
-        <v>27200</v>
+        <f t="shared" si="2"/>
+        <v>9550</v>
       </c>
       <c r="E33">
         <v>5</v>
       </c>
+      <c r="F33">
+        <v>3.8</v>
+      </c>
+      <c r="G33">
+        <v>1.8</v>
+      </c>
       <c r="H33" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>168633.9</v>
       </c>
       <c r="I33">
         <v>1</v>
@@ -3043,24 +3052,21 @@
       </c>
       <c r="S33">
         <v>0</v>
-      </c>
-      <c r="T33" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C34" s="2">
-        <v>3250</v>
+        <v>2000</v>
       </c>
       <c r="D34" s="2">
-        <f t="shared" ref="D34:D35" si="2">C34*E34</f>
-        <v>19500</v>
+        <f t="shared" ref="D34:D35" si="4">C34*E34</f>
+        <v>12000</v>
       </c>
       <c r="E34">
         <v>6</v>
@@ -3072,8 +3078,8 @@
         <v>1.5</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" ref="H34:H35" si="3">D34*9.81*G34</f>
-        <v>286942.5</v>
+        <f t="shared" ref="H34:H35" si="5">D34*9.81*G34</f>
+        <v>176580</v>
       </c>
       <c r="I34">
         <v>1</v>
@@ -3111,17 +3117,17 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C35" s="2">
-        <v>1910</v>
+        <v>1320</v>
       </c>
       <c r="D35" s="2">
-        <f t="shared" si="2"/>
-        <v>9550</v>
+        <f t="shared" si="4"/>
+        <v>6600</v>
       </c>
       <c r="E35">
         <v>5</v>
@@ -3133,8 +3139,8 @@
         <v>1.8</v>
       </c>
       <c r="H35" s="2">
-        <f t="shared" si="3"/>
-        <v>168633.9</v>
+        <f t="shared" si="5"/>
+        <v>116542.8</v>
       </c>
       <c r="I35">
         <v>1</v>
@@ -3172,33 +3178,23 @@
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>82</v>
-      </c>
-      <c r="B36" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C36" s="2">
-        <v>2000</v>
+        <v>1650</v>
       </c>
       <c r="D36" s="2">
-        <f t="shared" ref="D36:D37" si="4">C36*E36</f>
-        <v>12000</v>
+        <v>8300</v>
       </c>
       <c r="E36">
-        <v>6</v>
-      </c>
-      <c r="F36">
-        <v>3.7</v>
-      </c>
-      <c r="G36">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" ref="H36:H37" si="5">D36*9.81*G36</f>
-        <v>176580</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="I36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36">
         <v>0</v>
@@ -3219,7 +3215,7 @@
         <v>0</v>
       </c>
       <c r="P36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q36">
         <v>0</v>
@@ -3229,37 +3225,30 @@
       </c>
       <c r="S36">
         <v>0</v>
+      </c>
+      <c r="T36" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>82</v>
-      </c>
-      <c r="B37" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="C37" s="2">
-        <v>1320</v>
+        <v>1720</v>
       </c>
       <c r="D37" s="2">
-        <f t="shared" si="4"/>
-        <v>6600</v>
+        <v>8500</v>
       </c>
       <c r="E37">
-        <v>5</v>
-      </c>
-      <c r="F37">
-        <v>3.8</v>
-      </c>
-      <c r="G37">
-        <v>1.8</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="5"/>
-        <v>116542.8</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="I37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37">
         <v>0</v>
@@ -3280,7 +3269,7 @@
         <v>0</v>
       </c>
       <c r="P37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q37">
         <v>0</v>
@@ -3290,24 +3279,36 @@
       </c>
       <c r="S37">
         <v>0</v>
+      </c>
+      <c r="T37" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C38" s="2">
-        <v>1650</v>
+        <v>3023</v>
       </c>
       <c r="D38" s="2">
-        <v>8300</v>
+        <v>9070</v>
       </c>
       <c r="E38">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="F38">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G38">
+        <v>2.4</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D38*9.81*G38</f>
+        <v>213544.08000000002</v>
       </c>
       <c r="I38">
         <v>0</v>
@@ -3328,7 +3329,7 @@
         <v>0</v>
       </c>
       <c r="O38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P38">
         <v>0</v>
@@ -3343,25 +3344,34 @@
         <v>0</v>
       </c>
       <c r="T38" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C39" s="2">
-        <v>1720</v>
+        <v>2237</v>
       </c>
       <c r="D39" s="2">
-        <v>8500</v>
+        <v>6710</v>
       </c>
       <c r="E39">
-        <v>4.9000000000000004</v>
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G39">
+        <v>2.4</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D39*9.81*G39</f>
+        <v>157980.24000000002</v>
       </c>
       <c r="I39">
         <v>0</v>
@@ -3382,7 +3392,7 @@
         <v>0</v>
       </c>
       <c r="O39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P39">
         <v>0</v>
@@ -3397,24 +3407,18 @@
         <v>0</v>
       </c>
       <c r="T39" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40" s="2">
-        <v>3023</v>
+        <v>8</v>
       </c>
       <c r="D40" s="2">
-        <v>9070</v>
-      </c>
-      <c r="E40">
-        <v>3</v>
+        <v>4583.232</v>
       </c>
       <c r="F40">
         <v>4.5999999999999996</v>
@@ -3424,60 +3428,18 @@
       </c>
       <c r="H40" s="2">
         <f>D40*9.81*G40</f>
-        <v>213544.08000000002</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-      <c r="M40">
-        <v>0</v>
-      </c>
-      <c r="N40">
-        <v>0</v>
-      </c>
-      <c r="O40">
-        <v>1</v>
-      </c>
-      <c r="P40">
-        <v>0</v>
-      </c>
-      <c r="Q40">
-        <v>0</v>
-      </c>
-      <c r="R40">
-        <v>0</v>
-      </c>
-      <c r="S40">
-        <v>0</v>
-      </c>
-      <c r="T40" t="s">
-        <v>60</v>
+        <v>107907.614208</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="2">
-        <v>2237</v>
+        <v>9</v>
       </c>
       <c r="D41" s="2">
-        <v>6710</v>
-      </c>
-      <c r="E41">
-        <v>3</v>
+        <v>8436.6</v>
       </c>
       <c r="F41">
         <v>4.5999999999999996</v>
@@ -3486,55 +3448,19 @@
         <v>2.4</v>
       </c>
       <c r="H41" s="2">
-        <f>D41*9.81*G41</f>
-        <v>157980.24000000002</v>
-      </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="J41">
-        <v>0</v>
-      </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <v>0</v>
-      </c>
-      <c r="N41">
-        <v>0</v>
-      </c>
-      <c r="O41">
-        <v>1</v>
-      </c>
-      <c r="P41">
-        <v>0</v>
-      </c>
-      <c r="Q41">
-        <v>0</v>
-      </c>
-      <c r="R41">
-        <v>0</v>
-      </c>
-      <c r="S41">
-        <v>0</v>
-      </c>
-      <c r="T41" t="s">
-        <v>58</v>
+        <f t="shared" ref="H41:H49" si="6">D41*9.81*G41</f>
+        <v>198631.31039999999</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D42" s="2">
-        <v>4583.232</v>
+        <v>5689.8</v>
       </c>
       <c r="F42">
         <v>4.5999999999999996</v>
@@ -3543,64 +3469,130 @@
         <v>2.4</v>
       </c>
       <c r="H42" s="2">
-        <f>D42*9.81*G42</f>
-        <v>107907.614208</v>
+        <f t="shared" si="6"/>
+        <v>133960.65119999999</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>79</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>9</v>
+        <v>61</v>
+      </c>
+      <c r="C43" s="2">
+        <v>5443</v>
       </c>
       <c r="D43" s="2">
-        <v>8436.6</v>
-      </c>
-      <c r="F43">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="G43">
-        <v>2.4</v>
+        <v>27215</v>
+      </c>
+      <c r="E43">
+        <v>5</v>
       </c>
       <c r="H43" s="2">
-        <f t="shared" ref="H43:H51" si="6">D43*9.81*G43</f>
-        <v>198631.31039999999</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <v>0</v>
+      </c>
+      <c r="S43">
+        <v>0</v>
+      </c>
+      <c r="T43" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>80</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>10</v>
+        <v>62</v>
+      </c>
+      <c r="C44" s="2">
+        <v>2000</v>
       </c>
       <c r="D44" s="2">
-        <v>5689.8</v>
-      </c>
-      <c r="F44">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="G44">
-        <v>2.4</v>
+        <v>3500</v>
+      </c>
+      <c r="E44">
+        <v>1.75</v>
       </c>
       <c r="H44" s="2">
         <f t="shared" si="6"/>
-        <v>133960.65119999999</v>
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <v>0</v>
+      </c>
+      <c r="S44">
+        <v>0</v>
+      </c>
+      <c r="T44" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C45" s="2">
-        <v>5443</v>
+        <v>3575</v>
       </c>
       <c r="D45" s="2">
-        <v>27215</v>
+        <v>14300</v>
       </c>
       <c r="E45">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H45" s="2">
         <f t="shared" si="6"/>
@@ -3640,21 +3632,21 @@
         <v>0</v>
       </c>
       <c r="T45" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C46" s="2">
-        <v>2000</v>
+        <v>1625</v>
       </c>
       <c r="D46" s="2">
-        <v>3500</v>
+        <v>6500</v>
       </c>
       <c r="E46">
-        <v>1.75</v>
+        <v>4</v>
       </c>
       <c r="H46" s="2">
         <f t="shared" si="6"/>
@@ -3694,21 +3686,21 @@
         <v>0</v>
       </c>
       <c r="T46" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C47" s="2">
-        <v>3575</v>
+        <v>2000</v>
       </c>
       <c r="D47" s="2">
-        <v>14300</v>
+        <v>3500</v>
       </c>
       <c r="E47">
-        <v>4</v>
+        <v>1.75</v>
       </c>
       <c r="H47" s="2">
         <f t="shared" si="6"/>
@@ -3748,21 +3740,23 @@
         <v>0</v>
       </c>
       <c r="T47" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C48" s="2">
-        <v>1625</v>
+        <f>D48/E48</f>
+        <v>621.85757972913939</v>
       </c>
       <c r="D48" s="2">
-        <v>6500</v>
+        <f>3*3558.58/9.81</f>
+        <v>1088.2507645259939</v>
       </c>
       <c r="E48">
-        <v>4</v>
+        <v>1.75</v>
       </c>
       <c r="H48" s="2">
         <f t="shared" si="6"/>
@@ -3802,21 +3796,21 @@
         <v>0</v>
       </c>
       <c r="T48" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C49" s="2">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="D49" s="2">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="E49">
-        <v>1.75</v>
+        <v>4</v>
       </c>
       <c r="H49" s="2">
         <f t="shared" si="6"/>
@@ -3856,153 +3850,53 @@
         <v>0</v>
       </c>
       <c r="T49" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="C50" s="2">
-        <f>D50/E50</f>
-        <v>621.85757972913939</v>
+        <v>750</v>
       </c>
       <c r="D50" s="2">
-        <f>3*3558.58/9.81</f>
-        <v>1088.2507645259939</v>
+        <f>C50*E50</f>
+        <v>1724.9999999999998</v>
       </c>
       <c r="E50">
-        <v>1.75</v>
-      </c>
-      <c r="H50" s="2">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I50">
-        <v>0</v>
-      </c>
-      <c r="J50">
-        <v>0</v>
-      </c>
-      <c r="K50">
-        <v>0</v>
-      </c>
-      <c r="L50">
-        <v>0</v>
-      </c>
-      <c r="M50">
-        <v>0</v>
-      </c>
-      <c r="N50">
-        <v>0</v>
-      </c>
-      <c r="O50">
-        <v>0</v>
-      </c>
-      <c r="P50">
-        <v>0</v>
-      </c>
-      <c r="Q50">
-        <v>0</v>
-      </c>
-      <c r="R50">
-        <v>0</v>
-      </c>
-      <c r="S50">
-        <v>0</v>
-      </c>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H50" s="2"/>
       <c r="T50" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>72</v>
-      </c>
+      <c r="A51" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="1"/>
       <c r="C51" s="2">
-        <v>1000</v>
+        <v>750</v>
       </c>
       <c r="D51" s="2">
-        <v>4000</v>
+        <f>750*4</f>
+        <v>3000</v>
       </c>
       <c r="E51">
         <v>4</v>
       </c>
-      <c r="H51" s="2">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I51">
-        <v>0</v>
-      </c>
-      <c r="J51">
-        <v>0</v>
-      </c>
-      <c r="K51">
-        <v>0</v>
-      </c>
-      <c r="L51">
-        <v>0</v>
-      </c>
-      <c r="M51">
-        <v>0</v>
-      </c>
-      <c r="N51">
-        <v>0</v>
-      </c>
-      <c r="O51">
-        <v>0</v>
-      </c>
-      <c r="P51">
-        <v>0</v>
-      </c>
-      <c r="Q51">
-        <v>0</v>
-      </c>
-      <c r="R51">
-        <v>0</v>
-      </c>
-      <c r="S51">
-        <v>0</v>
-      </c>
-      <c r="T51" t="s">
-        <v>73</v>
-      </c>
+      <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>87</v>
-      </c>
-      <c r="C52" s="2">
-        <v>750</v>
-      </c>
-      <c r="D52" s="2">
-        <f>C52*E52</f>
-        <v>1724.9999999999998</v>
-      </c>
-      <c r="E52">
-        <v>2.2999999999999998</v>
-      </c>
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
       <c r="H52" s="2"/>
-      <c r="T52" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>88</v>
-      </c>
+      <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-      <c r="C53" s="2">
-        <v>750</v>
-      </c>
-      <c r="D53" s="2">
-        <f>750*4</f>
-        <v>3000</v>
-      </c>
-      <c r="E53">
-        <v>4</v>
-      </c>
       <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
@@ -4044,16 +3938,6 @@
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="H61" s="2"/>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="H62" s="2"/>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="H63" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>